<commit_message>
Unify the Data Preparation format
</commit_message>
<xml_diff>
--- a/01_Input/01_ClassificationTraining_DataPreparation.xlsx
+++ b/01_Input/01_ClassificationTraining_DataPreparation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Branches\WEFN\01_RawData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Branches\WEFN\01_Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5E1F2E5-4A04-4470-B481-A387527CC673}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AB9E0F-F921-46F1-B172-51F21934A498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -178,10 +178,6 @@
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
   <si>
-    <t>Year</t>
-    <phoneticPr fontId="19" type="noConversion"/>
-  </si>
-  <si>
     <t>Population</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
@@ -255,6 +251,10 @@
   </si>
   <si>
     <t>Active Working Population in Agriculture Percentage (%)</t>
+    <phoneticPr fontId="19" type="noConversion"/>
+  </si>
+  <si>
+    <t>Note</t>
     <phoneticPr fontId="19" type="noConversion"/>
   </si>
 </sst>
@@ -266,7 +266,7 @@
     <numFmt numFmtId="176" formatCode="0.0000"/>
     <numFmt numFmtId="177" formatCode="0.000"/>
   </numFmts>
-  <fonts count="24">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -896,7 +896,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -926,6 +926,15 @@
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1285,25 +1294,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B23" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G2" sqref="G2:G37"/>
+      <selection pane="bottomRight" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="10.33203125" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="12" width="8.77734375" customWidth="1"/>
-    <col min="14" max="14" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="10.375" customWidth="1"/>
+    <col min="6" max="6" width="11.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.375" customWidth="1"/>
+    <col min="8" max="8" width="12.75" customWidth="1"/>
+    <col min="9" max="12" width="8.75" customWidth="1"/>
+    <col min="14" max="14" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -1341,7 +1350,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1380,7 +1389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1419,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1458,7 +1467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1497,7 +1506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -1536,7 +1545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1575,7 +1584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>1</v>
       </c>
@@ -1614,7 +1623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1653,7 +1662,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -1692,7 +1701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1731,7 +1740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1770,7 +1779,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -1809,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -1848,7 +1857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1887,7 +1896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1926,7 +1935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -1965,7 +1974,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>3</v>
       </c>
@@ -2004,7 +2013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>41</v>
       </c>
@@ -2043,7 +2052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -2082,9 +2091,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" s="5">
         <v>8726.2804965044907</v>
@@ -2121,7 +2130,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -2160,7 +2169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -2199,7 +2208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -2238,7 +2247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -2277,7 +2286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -2318,7 +2327,7 @@
       </c>
       <c r="N26" s="6"/>
     </row>
-    <row r="27" spans="1:14">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -2357,7 +2366,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -2396,7 +2405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>4</v>
       </c>
@@ -2435,7 +2444,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:14">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>16</v>
       </c>
@@ -2474,7 +2483,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:14">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>17</v>
       </c>
@@ -2513,7 +2522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:14">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -2552,7 +2561,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>15</v>
       </c>
@@ -2591,9 +2600,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B34" s="5">
         <v>1785.2406124982001</v>
@@ -2630,7 +2639,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -2669,7 +2678,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -2708,9 +2717,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B37" s="5">
         <v>2276.2874505211598</v>
@@ -2762,17 +2771,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78054FFB-0FC1-404F-8536-4A80A54A69F6}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="63.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="70.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.125" style="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -2780,134 +2790,134 @@
         <v>45</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="D1" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>32</v>
       </c>
       <c r="B2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="11">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3" t="s">
         <v>51</v>
       </c>
-      <c r="C2">
-        <v>2012</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C3" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C3">
+      <c r="D3" s="11">
         <v>2003</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>33</v>
       </c>
       <c r="B4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C4">
+        <v>66</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="11">
         <v>2012</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="11">
         <v>2012</v>
       </c>
-      <c r="D5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6">
+        <v>62</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="11">
         <v>2012</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
-      </c>
-      <c r="C7">
+        <v>63</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="11">
         <v>2012</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" s="7" customFormat="1">
+    </row>
+    <row r="8" spans="1:4" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>44</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="7">
+        <v>48</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="12">
         <v>2012</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9">
+        <v>65</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="11">
         <v>2012</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{A7146BE5-EF42-42A1-AC31-27F10D420D1C}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{0E32973A-DED0-45A3-9388-05F2F1472BBF}"/>
-    <hyperlink ref="D4" r:id="rId3" xr:uid="{F6364954-13BD-4B3C-99CB-B9E03833ABB1}"/>
-    <hyperlink ref="D6" r:id="rId4" location="data/TP" xr:uid="{A9353E61-3827-4843-99EE-7692F3174CDB}"/>
-    <hyperlink ref="D7" r:id="rId5" location="data/TP" xr:uid="{CC854199-35F0-46AB-A21B-469A2039C19C}"/>
-    <hyperlink ref="D8" r:id="rId6" xr:uid="{5974CCD7-22A7-4112-8685-063FF9C35436}"/>
-    <hyperlink ref="D9" r:id="rId7" xr:uid="{88B952DC-725A-49B1-A1D9-0DAF40796F37}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{A7146BE5-EF42-42A1-AC31-27F10D420D1C}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{0E32973A-DED0-45A3-9388-05F2F1472BBF}"/>
+    <hyperlink ref="C4" r:id="rId3" xr:uid="{F6364954-13BD-4B3C-99CB-B9E03833ABB1}"/>
+    <hyperlink ref="C6" r:id="rId4" location="data/TP" xr:uid="{A9353E61-3827-4843-99EE-7692F3174CDB}"/>
+    <hyperlink ref="C7" r:id="rId5" location="data/TP" xr:uid="{CC854199-35F0-46AB-A21B-469A2039C19C}"/>
+    <hyperlink ref="C8" r:id="rId6" xr:uid="{5974CCD7-22A7-4112-8685-063FF9C35436}"/>
+    <hyperlink ref="C9" r:id="rId7" xr:uid="{88B952DC-725A-49B1-A1D9-0DAF40796F37}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>